<commit_message>
Relation of BI DAX
</commit_message>
<xml_diff>
--- a/Stock BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Stock BI by IM from Source).xlsx
+++ b/Stock BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Stock BI by IM from Source).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Imam Hossain\IDoc\Power BI by IM\Stock BI Report by Imam Hossain With Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DFC2EF-E0AD-41C5-AE1B-69E00B08F9C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B93BD37-57D2-40E9-8D24-D5780D064BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar Date" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="1. Stock Ageing" sheetId="3" r:id="rId3"/>
     <sheet name="Datediff()" sheetId="4" r:id="rId4"/>
     <sheet name="Calculate()" sheetId="5" r:id="rId5"/>
+    <sheet name="Relation of BI DAX" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>https://debug.to/899/calendarauto-function-can-not-find-a-base-column-of-datetime-type-in-the-model</t>
   </si>
@@ -2122,6 +2123,12 @@
   </si>
   <si>
     <t>https://www.datacamp.com/tutorial/power-bi-calculate-tutorial</t>
+  </si>
+  <si>
+    <t>Create and manage relationships in Power BI Desktop</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/en-us/power-bi/transform-model/desktop-create-and-manage-relationships</t>
   </si>
 </sst>
 </file>
@@ -2602,6 +2609,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>607314</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>84588</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E4ACD36-0526-1A9E-309B-826A05DF9D37}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="704850"/>
+          <a:ext cx="18285714" cy="9095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3358,7 +3414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4944380F-9D84-47EE-BCF8-56EB84A34E31}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -3382,4 +3438,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33DE77A-D502-468D-8D63-A6D26CB3AF1A}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Stock BI Report by Imam Hossain With Source\9. Yarn Stock Ageing
</commit_message>
<xml_diff>
--- a/Stock BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Stock BI by IM from Source).xlsx
+++ b/Stock BI Report by Imam Hossain With Source/Code, Code Flow, Function with Notes, Learning Source (Stock BI by IM from Source).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Imam Hossain\IDoc\Power BI by IM\Stock BI Report by Imam Hossain With Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B93BD37-57D2-40E9-8D24-D5780D064BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D05733B-6AFE-4384-8395-588348257377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="6" xr2:uid="{BA506BA8-62E4-42EB-93AD-9835F75A9973}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar Date" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Datediff()" sheetId="4" r:id="rId4"/>
     <sheet name="Calculate()" sheetId="5" r:id="rId5"/>
     <sheet name="Relation of BI DAX" sheetId="6" r:id="rId6"/>
+    <sheet name="Edit Interaction" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>https://debug.to/899/calendarauto-function-can-not-find-a-base-column-of-datetime-type-in-the-model</t>
   </si>
@@ -2129,13 +2131,22 @@
   </si>
   <si>
     <t>https://learn.microsoft.com/en-us/power-bi/transform-model/desktop-create-and-manage-relationships</t>
+  </si>
+  <si>
+    <t>How to Edit Interactions Between Visuals in Power Bi</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ENuG2F-tce0</t>
+  </si>
+  <si>
+    <t>In this video we will cover how to edit interactions between visuals in Power BI. We will cover how to cross highlight and how to filter visuals based on selections made in other visuals.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2192,6 +2203,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF131313"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2381,7 +2398,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2444,6 +2461,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2613,16 +2631,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>607314</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>84588</xdr:rowOff>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>254889</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>56013</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2645,8 +2663,145 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="704850"/>
+          <a:off x="9401175" y="295275"/>
           <a:ext cx="18285714" cy="9095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>456076</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>189819</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9378230-C9E9-DE67-F723-0EAB86D0EE8C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="647700"/>
+          <a:ext cx="8990476" cy="5447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>255547</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>122889</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18782CAF-63F7-7D7E-FCCA-4DF2D2C537AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4305300" y="257175"/>
+          <a:ext cx="13019047" cy="7485714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>455475</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>189288</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{682B16E9-4220-B487-C38D-C7580BC4E3D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="66675" y="2305050"/>
+          <a:ext cx="13800000" cy="9695238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2958,7 +3113,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3125,8 +3280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC4226C-7EF8-493E-A17B-893528C5BC34}">
   <dimension ref="B1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3156,8 +3311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCEA66B-EE88-40D3-8C3B-2968A700D0A6}">
   <dimension ref="A2:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3379,7 +3534,7 @@
   <dimension ref="B1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3390,7 +3545,7 @@
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="29" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3405,8 +3560,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{52D8A49B-B46E-4A79-A9AA-32DB1BAE58E5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3415,7 +3573,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3444,8 +3602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33DE77A-D502-468D-8D63-A6D26CB3AF1A}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3464,4 +3622,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F632628-7974-4F7D-A9AA-B6EEDB405C37}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2172347E-957E-473A-A572-DC1F11BB6C8F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>